<commit_message>
Updated webapp to support OT protocol generation from sample data.
</commit_message>
<xml_diff>
--- a/data/example_sample_file.xlsx
+++ b/data/example_sample_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neilswainston/git/liv-covid19/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F060597-DB5E-FD44-95BC-E61081425062}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA9D49B-8375-154A-A55E-A9813A08088E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="20340" windowHeight="16840" xr2:uid="{744BDF75-25B1-5041-9A3E-68996CDE714F}"/>
   </bookViews>
@@ -515,7 +515,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="A2" sqref="A2:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -545,6 +545,9 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>4920</v>
+      </c>
       <c r="B2" t="s">
         <v>35</v>
       </c>
@@ -701,6 +704,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>4920</v>
+      </c>
       <c r="B11" t="s">
         <v>36</v>
       </c>
@@ -833,6 +839,9 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>4920</v>
+      </c>
       <c r="B20" t="s">
         <v>37</v>
       </c>
@@ -962,6 +971,9 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>4920</v>
+      </c>
       <c r="B29" t="s">
         <v>38</v>
       </c>
@@ -1004,6 +1016,9 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>4920</v>
+      </c>
       <c r="B32" t="s">
         <v>39</v>
       </c>
@@ -1011,7 +1026,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>4920</v>
+      </c>
       <c r="B33" t="s">
         <v>40</v>
       </c>

</xml_diff>